<commit_message>
name change and minor edit to excel
</commit_message>
<xml_diff>
--- a/Output workbooks/international_migration_calculations.xlsx
+++ b/Output workbooks/international_migration_calculations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://centreforcities.sharepoint.com/sites/CentreForCities3/Shared Documents/Research/Social and Demographics/Escape to the Country/Data/Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M.Lange\Documents\GitHub\urban-population-internal-migration\Output workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="8_{014F7B3C-A698-4537-BD67-7ABAC580BA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54C7C970-7A67-4268-BFA2-0AA0CC0BCDE8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B59029E-C063-4DDB-A50F-5624A9B261D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculations" sheetId="2" r:id="rId1"/>
@@ -161,13 +161,13 @@
     <t>Copied from left</t>
   </si>
   <si>
-    <t>Pasted from 2024-02-15_Internal_migration</t>
-  </si>
-  <si>
-    <t>Pasted from 2024-01-25urbanpopulationcalculations</t>
-  </si>
-  <si>
-    <t>Pasted from 2024_02_21_Natural Increase</t>
+    <t>Pasted from internal migration statistics</t>
+  </si>
+  <si>
+    <t>Pasted from urban population statistics</t>
+  </si>
+  <si>
+    <t>Pasted from natural increase data</t>
   </si>
 </sst>
 </file>
@@ -2406,7 +2406,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2953,7 +2953,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61E1CBCD-14BF-4BD4-8E36-205EEC4F3FC0}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3741,14 +3743,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7a436561-34c6-48a8-833e-99c650fd3fe3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="25475540-9773-43a3-8df6-094be5ca1716" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4007,21 +4007,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7a436561-34c6-48a8-833e-99c650fd3fe3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="25475540-9773-43a3-8df6-094be5ca1716" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD23202E-E346-4106-AEFC-1EE081E8C743}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{864AF008-90A8-4B00-98B1-FADC393CEFAE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7a436561-34c6-48a8-833e-99c650fd3fe3"/>
-    <ds:schemaRef ds:uri="25475540-9773-43a3-8df6-094be5ca1716"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4046,9 +4045,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{864AF008-90A8-4B00-98B1-FADC393CEFAE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD23202E-E346-4106-AEFC-1EE081E8C743}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7a436561-34c6-48a8-833e-99c650fd3fe3"/>
+    <ds:schemaRef ds:uri="25475540-9773-43a3-8df6-094be5ca1716"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>